<commit_message>
P-W compatible with tap changers
</commit_message>
<xml_diff>
--- a/Datax.xlsx
+++ b/Datax.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\TFG\Codi\Tests\Tests_18_03_24_03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\TFG\Codi\Tests\Tests_25_03_01_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>R</t>
   </si>
@@ -108,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +395,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.06</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -447,14 +448,17 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>-0.1</v>
+      <c r="B3" s="2">
+        <v>-2</v>
       </c>
       <c r="C3">
-        <v>-0.05</v>
+        <v>-0.5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -465,32 +469,15 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
         <v>0</v>
       </c>
     </row>
@@ -530,10 +517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,33 +553,33 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.22</v>
+        <v>0.04</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D3">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -600,42 +587,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>0.1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>